<commit_message>
added config json file
</commit_message>
<xml_diff>
--- a/EC2_Config.ps1.xlsx
+++ b/EC2_Config.ps1.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\scripts\git_scripts\aws-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623A95AA-6A0B-4486-B79E-9B4D88E018F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62FF7B8-6183-4B87-B09C-136C9E7273FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37185" yWindow="4860" windowWidth="29670" windowHeight="15345" xr2:uid="{7374E4AC-EC4C-43CC-BB10-7730B7FDC2E1}"/>
+    <workbookView xWindow="2340" yWindow="0" windowWidth="21600" windowHeight="15585" activeTab="2" xr2:uid="{7374E4AC-EC4C-43CC-BB10-7730B7FDC2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="EC2_Instances" sheetId="1" r:id="rId1"/>
+    <sheet name="EBS_Volumes" sheetId="2" r:id="rId2"/>
+    <sheet name="SG_Rules" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
   <si>
     <t>AccountName</t>
   </si>
@@ -192,6 +197,129 @@
   </si>
   <si>
     <t>hostname=autotest-vm;solution=script_test</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>VolumeName</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>VolumeType</t>
+  </si>
+  <si>
+    <t>VolumeMount</t>
+  </si>
+  <si>
+    <t>VolumeLabel</t>
+  </si>
+  <si>
+    <t>Iops</t>
+  </si>
+  <si>
+    <t>Throughput</t>
+  </si>
+  <si>
+    <t>Encrypted</t>
+  </si>
+  <si>
+    <t>KmsKeyId</t>
+  </si>
+  <si>
+    <t>SnapshotId</t>
+  </si>
+  <si>
+    <t>MultiAttachEnabled</t>
+  </si>
+  <si>
+    <t>web-server-data-01</t>
+  </si>
+  <si>
+    <t>D:</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>ipf-aws-vmc-sddc1</t>
+  </si>
+  <si>
+    <t>sgID</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>GroupDescription</t>
+  </si>
+  <si>
+    <t>VpcId</t>
+  </si>
+  <si>
+    <t>RuleType</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>FromPort</t>
+  </si>
+  <si>
+    <t>ToPort</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>web-servers-sg</t>
+  </si>
+  <si>
+    <t>Security group for web servers</t>
+  </si>
+  <si>
+    <t>vpc-12345678</t>
+  </si>
+  <si>
+    <t>ingress</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>0.0.0.0/0</t>
+  </si>
+  <si>
+    <t>HTTP access from internet</t>
+  </si>
+  <si>
+    <t>Environment=prod</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>HTTPS access from internet</t>
+  </si>
+  <si>
+    <t>10.0.0.0/16</t>
+  </si>
+  <si>
+    <t>SSH access from VPC</t>
+  </si>
+  <si>
+    <t>egress</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>All outbound traffic</t>
   </si>
 </sst>
 </file>
@@ -248,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -258,6 +386,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -275,6 +422,45 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ec2_instances"/>
+      <sheetName val="ebs_volumes"/>
+      <sheetName val="sg_rules"/>
+      <sheetName val="lookup"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>InstanceName</v>
+          </cell>
+          <cell r="AH1" t="str">
+            <v>Tags</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="D2" t="str">
+            <v>az1autotest-vm</v>
+          </cell>
+          <cell r="AH2" t="str">
+            <v>hostname=autotest-vm;solution=script_test</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3449FCF0-41DE-4872-86E1-ADB9888097B5}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -831,4 +1017,356 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C228985C-789E-4966-9DC2-37BBAC45DA1E}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>[1]ec2_instances!$D$2</f>
+        <v>az1autotest-vm</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3">
+        <v>390439356506</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2">
+        <v>4000</v>
+      </c>
+      <c r="K2">
+        <v>250</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="str">
+        <f>_xlfn.XLOOKUP(A2,[1]ec2_instances!D:D,[1]ec2_instances!AH:AH)</f>
+        <v>hostname=autotest-vm;solution=script_test</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B29CD5-DE70-45D1-AB18-37C72B5B430C}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="9">
+        <v>80</v>
+      </c>
+      <c r="H2" s="9">
+        <v>80</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="10">
+        <v>390439356506</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="9">
+        <v>443</v>
+      </c>
+      <c r="H3" s="9">
+        <v>443</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="10">
+        <v>390439356506</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="9">
+        <v>22</v>
+      </c>
+      <c r="H4" s="9">
+        <v>22</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="10">
+        <v>390439356506</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>-1</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="10">
+        <v>390439356506</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit changes to excel file
</commit_message>
<xml_diff>
--- a/EC2_Config.ps1.xlsx
+++ b/EC2_Config.ps1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\aws-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D81D93-4498-4E9A-8F4E-9641019A68D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F87B34-1084-4343-8E90-CDF2D231217C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7374E4AC-EC4C-43CC-BB10-7730B7FDC2E1}"/>
   </bookViews>
@@ -742,7 +742,7 @@
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,6 +982,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>